<commit_message>
created route algo to deliver packages. Needs optimization
</commit_message>
<xml_diff>
--- a/Project/data/Distances.xlsx
+++ b/Project/data/Distances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lo850n/Desktop/Leo/CC950/WGU_C950/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95C248F-4C97-FC40-95FC-4395F0CFFA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5A649B-59A9-7646-B3CA-623E29672FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,10 +223,6 @@
  5383 South 900 East #104</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5383 S 900 East #104
-(84117)</t>
-  </si>
-  <si>
     <t>Rice Terrace Pavilion Park
  600 E 900 South</t>
   </si>
@@ -244,6 +240,10 @@
   </si>
   <si>
     <t>DISTANCE BETWEEN HUBS IN MILES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5383 South 900 East #104
+(84117)</t>
   </si>
 </sst>
 </file>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -881,7 +881,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="164" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="20" t="s">
@@ -960,10 +960,10 @@
         <v>48</v>
       </c>
       <c r="AB1" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="52" x14ac:dyDescent="0.2">
@@ -2411,7 +2411,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C26" s="4">
         <v>2.4</v>
@@ -2493,10 +2493,10 @@
     </row>
     <row r="27" spans="1:29" ht="26" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="C27" s="4">
         <v>5</v>
@@ -2580,10 +2580,10 @@
     </row>
     <row r="28" spans="1:29" ht="23.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>53</v>
       </c>
       <c r="C28" s="9">
         <v>3.6</v>
@@ -2674,15 +2674,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67abd11da167d8eab610c259a823e4c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d3ab84303ed41503c975572ff37e680" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3120,6 +3111,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3158,14 +3158,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83388E46-74FF-49C2-B8E6-3BEB0ECD2207}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3181,6 +3173,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>